<commit_message>
Commit working version for Colab. Have to refactor, test edge cases, incorporate schedule
</commit_message>
<xml_diff>
--- a/agg.xlsx
+++ b/agg.xlsx
@@ -16,15 +16,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>folder_1</t>
   </si>
   <si>
+    <t>file1.pdf</t>
+  </si>
+  <si>
+    <t>file2.pdf</t>
+  </si>
+  <si>
+    <t>file3.pdf</t>
+  </si>
+  <si>
+    <t>file4.pdf</t>
+  </si>
+  <si>
     <t>folder_2</t>
   </si>
   <si>
+    <t>file6.pdf</t>
+  </si>
+  <si>
+    <t>file5.pdf</t>
+  </si>
+  <si>
     <t>folder_3</t>
+  </si>
+  <si>
+    <t>file5 copia 2.pdf</t>
+  </si>
+  <si>
+    <t>file5 copia.pdf</t>
+  </si>
+  <si>
+    <t>.DS_Store</t>
+  </si>
+  <si>
+    <t>file4 copia.pdf</t>
+  </si>
+  <si>
+    <t>file6 copia 2.pdf</t>
+  </si>
+  <si>
+    <t>file4 copia 2.pdf</t>
+  </si>
+  <si>
+    <t>file6 copia.pdf</t>
   </si>
 </sst>
 </file>
@@ -382,30 +421,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -415,30 +495,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -448,30 +561,119 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>